<commit_message>
MATLAB: fixed matlab and excel files
</commit_message>
<xml_diff>
--- a/Testing/MatlabFitting/IRSensorTesting.xlsx
+++ b/Testing/MatlabFitting/IRSensorTesting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\GitHub\MECHENG-706-Part1\Testing\MatlabFitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E566C67-17BD-46F8-93EF-4FB8CA7CE914}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6CE8A41-1061-41F9-B41A-F2A62CDD1AEA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C9927716-11C2-4E11-8745-E6269F2EDD6B}"/>
+    <workbookView xWindow="-10665" yWindow="4770" windowWidth="21600" windowHeight="11385" xr2:uid="{C9927716-11C2-4E11-8745-E6269F2EDD6B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -397,23 +397,23 @@
   <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>